<commit_message>
ajuste no model produtos farmaceuticos
</commit_message>
<xml_diff>
--- a/dados/produto_daf.xlsx
+++ b/dados/produto_daf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ed001fd75dfbae91/Área de Trabalho/SisDAF/dados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{8C01042F-D150-4CC1-BA29-85551AD8AE4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49F68508-5AAF-4C0D-BEC9-5A5E7C07B17A}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{8C01042F-D150-4CC1-BA29-85551AD8AE4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD82C73C-BD54-45FF-B405-42661F0D5EB9}"/>
   <bookViews>
     <workbookView xWindow="10290" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5821,8 +5821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{718352EC-7F7A-431B-9250-49707EE5F3F5}">
   <dimension ref="A1:AR937"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="Q8" sqref="H8:Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>